<commit_message>
GUI Addition and scraper cleanup
</commit_message>
<xml_diff>
--- a/vendorList.xlsx
+++ b/vendorList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yhayashi\Documents\Yuki's Folder\Python\Web Scraper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6AFE139-9565-4F6F-8B6D-1204C225624D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB1EDD5-CE79-4BEE-B165-5030D2FD341C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="29">
   <si>
     <t>Vendor</t>
   </si>
@@ -70,6 +70,48 @@
   </si>
   <si>
     <t>https://www.timberland.ca/shop/VFSearchDisplay?catalogId=10102&amp;storeId=7121&amp;langId=-12&amp;searchTerm=_xxx_</t>
+  </si>
+  <si>
+    <t>searchID</t>
+  </si>
+  <si>
+    <t>searchWrapper</t>
+  </si>
+  <si>
+    <t>searchItem</t>
+  </si>
+  <si>
+    <t>imageWrapper</t>
+  </si>
+  <si>
+    <t>imageSrc</t>
+  </si>
+  <si>
+    <t>descWrapper</t>
+  </si>
+  <si>
+    <t>descSrc</t>
+  </si>
+  <si>
+    <t>main</t>
+  </si>
+  <si>
+    <t>link-wrapper</t>
+  </si>
+  <si>
+    <t>view-card select-item</t>
+  </si>
+  <si>
+    <t>image-wrapper mobile</t>
+  </si>
+  <si>
+    <t>data-src</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>p</t>
   </si>
 </sst>
 </file>
@@ -389,20 +431,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D3" sqref="D3:J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.21875" customWidth="1"/>
     <col min="2" max="2" width="24.6640625" customWidth="1"/>
-    <col min="3" max="3" width="17.109375" customWidth="1"/>
+    <col min="3" max="3" width="100" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -412,8 +461,29 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -423,8 +493,29 @@
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="D2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -434,8 +525,29 @@
       <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="D3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -445,8 +557,29 @@
       <c r="C4" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="D4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -455,6 +588,27 @@
       </c>
       <c r="C5" s="2" t="s">
         <v>14</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>